<commit_message>
Se completan escenario 13 y Escenario 21
</commit_message>
<xml_diff>
--- a/Cypress/Summary_Semana7.xlsx
+++ b/Cypress/Summary_Semana7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\PA_Semana5\Cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA08C00-FC67-4AD2-8E25-7345679A846B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DCF47-E872-4DF5-BA5A-F88345BE1CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{D6F45A50-01BB-42E3-84B2-F228A2D1A996}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D6F45A50-01BB-42E3-84B2-F228A2D1A996}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="20">
   <si>
     <t>Escenario</t>
   </si>
@@ -83,21 +83,29 @@
     <t>Estrategia de Generación</t>
   </si>
   <si>
-    <t>Incidencia</t>
-  </si>
-  <si>
     <t>Funcional</t>
   </si>
   <si>
     <t>Crear una nueva Pagina
 (Escenario 22)</t>
   </si>
+  <si>
+    <t>Incidencia #19</t>
+  </si>
+  <si>
+    <t>Agregar un nuevo Miembro
+(Escenario 13)</t>
+  </si>
+  <si>
+    <t>Crear un nuevo Tag
+(Escenario 21)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +123,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -147,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -347,10 +363,84 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -365,12 +455,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -394,9 +481,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -409,19 +493,46 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -738,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5194DC-AE4F-4D1F-959C-10FACBF13535}">
-  <dimension ref="A1:E122"/>
+  <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="J122" sqref="J122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,730 +866,941 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>16</v>
+      <c r="E3" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="10">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>16</v>
+      <c r="E4" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="10">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>16</v>
+      <c r="E5" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>16</v>
+      <c r="E6" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13" t="s">
-        <v>16</v>
+      <c r="E7" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>16</v>
+      <c r="E8" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>16</v>
+      <c r="E9" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>16</v>
+      <c r="E10" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="20" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="13" t="s">
-        <v>16</v>
+      <c r="E11" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="14" t="s">
-        <v>15</v>
+      <c r="E12" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="E16" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="15"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="E17" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
       <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="15"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="12">
+      <c r="E18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="15"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="15"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="E19" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="15"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="12">
+      <c r="E20" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="15"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="E21" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="15"/>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="18" t="s">
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="19"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="E23" s="18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+      <c r="B24" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="10">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="10">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="10">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="10">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="10">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="10">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
+      <c r="A37" s="10">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+      <c r="A38" s="10">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+      <c r="A39" s="10">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+      <c r="A40" s="10">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
+      <c r="A41" s="10">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
+      <c r="A42" s="10">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+      <c r="A43" s="10">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
+      <c r="B43" s="20"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="13">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="23" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="A45" s="7">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="B45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+      <c r="A46" s="10">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="A47" s="10">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="A48" s="10">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="A49" s="10">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="2"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="A50" s="10">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="20"/>
+      <c r="D50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="A51" s="10">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="20"/>
+      <c r="D51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
+      <c r="A52" s="10">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="20"/>
+      <c r="D52" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
+      <c r="A53" s="10">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
+      <c r="B53" s="20"/>
+      <c r="C53" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
+      <c r="A54" s="10">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
+      <c r="A55" s="10">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="2"/>
+      <c r="B55" s="20"/>
+      <c r="C55" s="20"/>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
+      <c r="A56" s="10">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="2"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="20"/>
+      <c r="D56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
+      <c r="A57" s="10">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="2"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="20"/>
+      <c r="D57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E57" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
+      <c r="A58" s="10">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
+      <c r="A59" s="10">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="2"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
+      <c r="A60" s="10">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="20"/>
+      <c r="D60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
+      <c r="A61" s="10">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="2"/>
+      <c r="B61" s="20"/>
+      <c r="C61" s="20"/>
+      <c r="D61" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
+      <c r="A62" s="10">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="20"/>
+      <c r="D62" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
+      <c r="A63" s="10">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="2"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="20"/>
+      <c r="D63" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
+      <c r="A64" s="10">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
+      <c r="B64" s="20"/>
+      <c r="C64" s="20"/>
+      <c r="D64" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E64" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="13">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+      <c r="D65" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" s="23" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
+      <c r="A66" s="3">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E66" s="3"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
@@ -1486,8 +1808,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E67" s="2"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,18 +1820,22 @@
         <v>66</v>
       </c>
       <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="2"/>
+      <c r="C68" s="20"/>
+      <c r="D68" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E68" s="2"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
-        <f t="shared" ref="A69:A122" si="1">A68+1</f>
+        <f t="shared" ref="A69:A128" si="1">A68+1</f>
         <v>67</v>
       </c>
       <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E69" s="2"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1516,8 +1844,10 @@
         <v>68</v>
       </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="2"/>
+      <c r="C70" s="20"/>
+      <c r="D70" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E70" s="2"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1526,8 +1856,10 @@
         <v>69</v>
       </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2"/>
+      <c r="C71" s="20"/>
+      <c r="D71" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E71" s="2"/>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,8 +1868,10 @@
         <v>70</v>
       </c>
       <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="C72" s="20"/>
+      <c r="D72" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E72" s="2"/>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1546,8 +1880,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="2"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E73" s="2"/>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1556,8 +1892,12 @@
         <v>72</v>
       </c>
       <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
+      <c r="C74" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E74" s="2"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,8 +1906,10 @@
         <v>73</v>
       </c>
       <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
+      <c r="C75" s="20"/>
+      <c r="D75" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E75" s="2"/>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1576,8 +1918,10 @@
         <v>74</v>
       </c>
       <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E76" s="2"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,8 +1930,10 @@
         <v>75</v>
       </c>
       <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="2"/>
+      <c r="C77" s="20"/>
+      <c r="D77" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E77" s="2"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -1596,8 +1942,10 @@
         <v>76</v>
       </c>
       <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E78" s="2"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -1606,8 +1954,10 @@
         <v>77</v>
       </c>
       <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E79" s="2"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -1616,8 +1966,12 @@
         <v>78</v>
       </c>
       <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
+      <c r="C80" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E80" s="2"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -1626,8 +1980,10 @@
         <v>79</v>
       </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="2"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E81" s="2"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,8 +1992,10 @@
         <v>80</v>
       </c>
       <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E82" s="2"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,8 +2004,10 @@
         <v>81</v>
       </c>
       <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
+      <c r="C83" s="20"/>
+      <c r="D83" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E83" s="2"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -1656,8 +2016,10 @@
         <v>82</v>
       </c>
       <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E84" s="2"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -1666,18 +2028,22 @@
         <v>83</v>
       </c>
       <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="2"/>
+      <c r="C85" s="20"/>
+      <c r="D85" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E85" s="2"/>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
       <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="E86" s="2"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -1686,8 +2052,12 @@
         <v>85</v>
       </c>
       <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
+      <c r="C87" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E87" s="2"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -1696,8 +2066,10 @@
         <v>86</v>
       </c>
       <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="C88" s="20"/>
+      <c r="D88" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E88" s="2"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -1706,8 +2078,10 @@
         <v>87</v>
       </c>
       <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="2"/>
+      <c r="C89" s="20"/>
+      <c r="D89" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E89" s="2"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,8 +2090,10 @@
         <v>88</v>
       </c>
       <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
+      <c r="C90" s="20"/>
+      <c r="D90" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E90" s="2"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -1726,8 +2102,10 @@
         <v>89</v>
       </c>
       <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="C91" s="20"/>
+      <c r="D91" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E91" s="2"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,8 +2114,10 @@
         <v>90</v>
       </c>
       <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
+      <c r="C92" s="20"/>
+      <c r="D92" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E92" s="2"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -1746,8 +2126,10 @@
         <v>91</v>
       </c>
       <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
+      <c r="C93" s="20"/>
+      <c r="D93" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E93" s="2"/>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,8 +2138,10 @@
         <v>92</v>
       </c>
       <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2"/>
+      <c r="C94" s="20"/>
+      <c r="D94" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E94" s="2"/>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -1766,8 +2150,12 @@
         <v>93</v>
       </c>
       <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="2"/>
+      <c r="C95" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E95" s="2"/>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,8 +2164,10 @@
         <v>94</v>
       </c>
       <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="2"/>
+      <c r="C96" s="20"/>
+      <c r="D96" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E96" s="2"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -1786,8 +2176,10 @@
         <v>95</v>
       </c>
       <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="2"/>
+      <c r="C97" s="20"/>
+      <c r="D97" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E97" s="2"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -1796,8 +2188,10 @@
         <v>96</v>
       </c>
       <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="2"/>
+      <c r="C98" s="20"/>
+      <c r="D98" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E98" s="2"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,8 +2200,10 @@
         <v>97</v>
       </c>
       <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="2"/>
+      <c r="C99" s="20"/>
+      <c r="D99" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E99" s="2"/>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -1816,8 +2212,10 @@
         <v>98</v>
       </c>
       <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
+      <c r="C100" s="20"/>
+      <c r="D100" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E100" s="2"/>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -1826,8 +2224,12 @@
         <v>99</v>
       </c>
       <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="2"/>
+      <c r="C101" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E101" s="2"/>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -1836,8 +2238,10 @@
         <v>100</v>
       </c>
       <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
+      <c r="C102" s="20"/>
+      <c r="D102" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E102" s="2"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -1846,8 +2250,10 @@
         <v>101</v>
       </c>
       <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
+      <c r="C103" s="20"/>
+      <c r="D103" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E103" s="2"/>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -1856,8 +2262,10 @@
         <v>102</v>
       </c>
       <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="2"/>
+      <c r="C104" s="20"/>
+      <c r="D104" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E104" s="2"/>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -1866,8 +2274,10 @@
         <v>103</v>
       </c>
       <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="2"/>
+      <c r="C105" s="20"/>
+      <c r="D105" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E105" s="2"/>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -1876,18 +2286,22 @@
         <v>104</v>
       </c>
       <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="2"/>
+      <c r="C106" s="20"/>
+      <c r="D106" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E106" s="2"/>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
       <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
+      <c r="C107" s="21"/>
+      <c r="D107" s="14" t="s">
+        <v>8</v>
+      </c>
       <c r="E107" s="2"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -1896,8 +2310,12 @@
         <v>106</v>
       </c>
       <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="2"/>
+      <c r="C108" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="E108" s="2"/>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,8 +2324,10 @@
         <v>107</v>
       </c>
       <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="2"/>
+      <c r="C109" s="20"/>
+      <c r="D109" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E109" s="2"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -1916,8 +2336,10 @@
         <v>108</v>
       </c>
       <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="2"/>
+      <c r="C110" s="20"/>
+      <c r="D110" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E110" s="2"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -1926,8 +2348,10 @@
         <v>109</v>
       </c>
       <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
+      <c r="C111" s="20"/>
+      <c r="D111" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E111" s="2"/>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -1936,8 +2360,10 @@
         <v>110</v>
       </c>
       <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="2"/>
+      <c r="C112" s="20"/>
+      <c r="D112" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E112" s="2"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -1946,8 +2372,10 @@
         <v>111</v>
       </c>
       <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
+      <c r="C113" s="20"/>
+      <c r="D113" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E113" s="2"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -1956,8 +2384,10 @@
         <v>112</v>
       </c>
       <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="2"/>
+      <c r="C114" s="20"/>
+      <c r="D114" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E114" s="2"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -1966,8 +2396,10 @@
         <v>113</v>
       </c>
       <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="2"/>
+      <c r="C115" s="20"/>
+      <c r="D115" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E115" s="2"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -1976,8 +2408,12 @@
         <v>114</v>
       </c>
       <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
+      <c r="C116" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E116" s="2"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -1986,8 +2422,10 @@
         <v>115</v>
       </c>
       <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
+      <c r="C117" s="20"/>
+      <c r="D117" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="E117" s="2"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -1996,8 +2434,10 @@
         <v>116</v>
       </c>
       <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="2"/>
+      <c r="C118" s="20"/>
+      <c r="D118" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E118" s="2"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -2006,8 +2446,10 @@
         <v>117</v>
       </c>
       <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="2"/>
+      <c r="C119" s="20"/>
+      <c r="D119" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="E119" s="2"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -2016,8 +2458,10 @@
         <v>118</v>
       </c>
       <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="2"/>
+      <c r="C120" s="20"/>
+      <c r="D120" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="E120" s="2"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -2025,27 +2469,122 @@
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="2"/>
+      <c r="B121" s="17"/>
+      <c r="C121" s="20"/>
+      <c r="D121" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E121" s="2"/>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="2">
+      <c r="A122" s="24">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
       <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="2"/>
+      <c r="C122" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E122" s="2"/>
     </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="24">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="25"/>
+      <c r="D123" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E123" s="2"/>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" s="24">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+      <c r="B124" s="2"/>
+      <c r="C124" s="25"/>
+      <c r="D124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E124" s="2"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="24">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+      <c r="B125" s="2"/>
+      <c r="C125" s="25"/>
+      <c r="D125" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E125" s="2"/>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A126" s="24">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+      <c r="B126" s="2"/>
+      <c r="C126" s="25"/>
+      <c r="D126" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126" s="2"/>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A127" s="24">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+      <c r="B127" s="2"/>
+      <c r="C127" s="25"/>
+      <c r="D127" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E127" s="2"/>
+    </row>
+    <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="24">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+      <c r="B128" s="2"/>
+      <c r="C128" s="26"/>
+      <c r="D128" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E128" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="21">
+    <mergeCell ref="C101:C107"/>
+    <mergeCell ref="C108:C115"/>
+    <mergeCell ref="C116:C121"/>
+    <mergeCell ref="C122:C128"/>
+    <mergeCell ref="C66:C73"/>
+    <mergeCell ref="C74:C79"/>
+    <mergeCell ref="C80:C86"/>
+    <mergeCell ref="C87:C94"/>
+    <mergeCell ref="C95:C100"/>
     <mergeCell ref="C3:C10"/>
     <mergeCell ref="C11:C16"/>
     <mergeCell ref="C17:C23"/>
     <mergeCell ref="B3:B23"/>
+    <mergeCell ref="C24:C31"/>
+    <mergeCell ref="C45:C52"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="C59:C65"/>
+    <mergeCell ref="B45:B65"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="B24:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Se completa entregable de la semana 7
</commit_message>
<xml_diff>
--- a/Cypress/Summary_Semana7.xlsx
+++ b/Cypress/Summary_Semana7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\PA_Semana5\Cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4DCF47-E872-4DF5-BA5A-F88345BE1CC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03334B9E-E494-48F5-9C1C-744D906E96C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D6F45A50-01BB-42E3-84B2-F228A2D1A996}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="27">
   <si>
     <t>Escenario</t>
   </si>
@@ -99,6 +99,30 @@
   <si>
     <t>Crear un nuevo Tag
 (Escenario 21)</t>
+  </si>
+  <si>
+    <t>Hacer LogIn
+(Escenario 0)</t>
+  </si>
+  <si>
+    <t>Crear un Post
+(Escenario 1)</t>
+  </si>
+  <si>
+    <t>Agregar un Miembro
+(Escenario 5)</t>
+  </si>
+  <si>
+    <t>Incidencia #20</t>
+  </si>
+  <si>
+    <t>Incidencia #21</t>
+  </si>
+  <si>
+    <t>Incidencia #22</t>
+  </si>
+  <si>
+    <t>Incidencia #23</t>
   </si>
 </sst>
 </file>
@@ -163,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -187,19 +211,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -413,10 +424,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -433,16 +444,66 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -455,7 +516,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -463,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -472,67 +533,85 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -851,13 +930,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5194DC-AE4F-4D1F-959C-10FACBF13535}">
   <dimension ref="A1:J128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J122" sqref="J122"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="25.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="31" style="1" customWidth="1"/>
     <col min="5" max="5" width="26.42578125" style="1" customWidth="1"/>
@@ -866,1704 +945,1851 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:5" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <f>A3+1</f>
         <v>2</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <f t="shared" ref="A5:A68" si="0">A4+1</f>
         <v>3</v>
       </c>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="10">
+      <c r="A9" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10">
+      <c r="A11" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20" t="s">
+      <c r="B11" s="19"/>
+      <c r="C11" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="10">
+      <c r="A12" s="9">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="10">
+      <c r="A13" s="9">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="10">
+      <c r="A14" s="9">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="10">
+      <c r="A15" s="9">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="9">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20" t="s">
+      <c r="A17" s="9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
+      <c r="A18" s="9">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="20"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
       <c r="D18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="15"/>
+      <c r="E18" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
+      <c r="A19" s="9">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10">
+      <c r="A20" s="9">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
+      <c r="A21" s="9">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="E21" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
+      <c r="A22" s="9">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="20"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="17" t="s">
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="17" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="C24" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
+      <c r="A25" s="9">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
+      <c r="A26" s="9">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="E26" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
+      <c r="A27" s="9">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="10">
+      <c r="A28" s="9">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="10">
+      <c r="A29" s="9">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E29" s="11" t="s">
+      <c r="E29" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="10">
+      <c r="A30" s="9">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="10">
+      <c r="A31" s="9">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="10">
+      <c r="A32" s="9">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="20" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="10">
+      <c r="A34" s="9">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="10">
+      <c r="A35" s="9">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E35" s="11" t="s">
+      <c r="E35" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
+      <c r="A36" s="9">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="20"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="11" t="s">
+      <c r="E36" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="10">
+      <c r="A37" s="9">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
+      <c r="A38" s="9">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="20" t="s">
+      <c r="B38" s="19"/>
+      <c r="C38" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="E38" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="10">
+      <c r="A39" s="9">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="10">
+      <c r="A40" s="9">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E40" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="10">
+      <c r="A41" s="9">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="11" t="s">
+      <c r="E41" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="10">
+      <c r="A42" s="9">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="20"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E42" s="11" t="s">
+      <c r="E42" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="10">
+      <c r="A43" s="9">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="20"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E43" s="11" t="s">
+      <c r="E43" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="13">
+      <c r="A44" s="12">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
-      <c r="D44" s="14" t="s">
+      <c r="B44" s="20"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+      <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B45" s="19" t="s">
+      <c r="B45" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="19" t="s">
+      <c r="C45" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D45" s="8" t="s">
+      <c r="D45" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E45" s="9" t="s">
+      <c r="E45" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="10">
+      <c r="A46" s="9">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="11" t="s">
+      <c r="E46" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="10">
+      <c r="A47" s="9">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E47" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="10">
+      <c r="A48" s="9">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="E48" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
+      <c r="A49" s="9">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="E49" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="10">
+      <c r="A50" s="9">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="E50" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
+      <c r="A51" s="9">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="E51" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="10">
+      <c r="A52" s="9">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="20"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="E52" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="10">
+      <c r="A53" s="9">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="20" t="s">
+      <c r="B53" s="19"/>
+      <c r="C53" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="E53" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="10">
+      <c r="A54" s="9">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="19"/>
       <c r="D54" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="E54" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="10">
+      <c r="A55" s="9">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B55" s="20"/>
-      <c r="C55" s="20"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
       <c r="D55" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E55" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="10">
+      <c r="A56" s="9">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="20"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E56" s="11" t="s">
+      <c r="E56" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="10">
+      <c r="A57" s="9">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="20"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="19"/>
       <c r="D57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E57" s="11" t="s">
+      <c r="E57" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="10">
+      <c r="A58" s="9">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E58" s="11" t="s">
+      <c r="E58" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="10">
+      <c r="A59" s="9">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="20" t="s">
+      <c r="B59" s="19"/>
+      <c r="C59" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E59" s="11" t="s">
+      <c r="E59" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="10">
+      <c r="A60" s="9">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="20"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="19"/>
       <c r="D60" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E60" s="11" t="s">
+      <c r="E60" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="10">
+      <c r="A61" s="9">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="20"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="19"/>
       <c r="D61" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E61" s="11" t="s">
+      <c r="E61" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="10">
+      <c r="A62" s="9">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="20"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E62" s="11" t="s">
+      <c r="E62" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="10">
+      <c r="A63" s="9">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="20"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E63" s="11" t="s">
+      <c r="E63" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="10">
+      <c r="A64" s="9">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="20"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E64" s="11" t="s">
+      <c r="E64" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="13">
+      <c r="A65" s="12">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B65" s="21"/>
-      <c r="C65" s="21"/>
-      <c r="D65" s="14" t="s">
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="23" t="s">
+      <c r="E65" s="18" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+      <c r="A66" s="6">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="19" t="s">
+      <c r="B66" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D66" s="8" t="s">
+      <c r="D66" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E66" s="3"/>
+      <c r="E66" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
+      <c r="A67" s="9">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B67" s="2"/>
-      <c r="C67" s="20"/>
+      <c r="B67" s="26"/>
+      <c r="C67" s="19"/>
       <c r="D67" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
+      <c r="A68" s="9">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B68" s="2"/>
-      <c r="C68" s="20"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="19"/>
       <c r="D68" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2">
+      <c r="A69" s="9">
         <f t="shared" ref="A69:A128" si="1">A68+1</f>
         <v>67</v>
       </c>
-      <c r="B69" s="2"/>
-      <c r="C69" s="20"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="19"/>
       <c r="D69" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2">
+      <c r="A70" s="9">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B70" s="2"/>
-      <c r="C70" s="20"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+      <c r="A71" s="9">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="20"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="19"/>
       <c r="D71" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2">
+      <c r="A72" s="9">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="20"/>
+      <c r="B72" s="26"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E72" s="2"/>
+      <c r="E72" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2">
+      <c r="A73" s="9">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B73" s="2"/>
-      <c r="C73" s="20"/>
+      <c r="B73" s="26"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E73" s="2"/>
+      <c r="E73" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2">
+      <c r="A74" s="9">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B74" s="2"/>
-      <c r="C74" s="20" t="s">
+      <c r="B74" s="26"/>
+      <c r="C74" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D74" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2">
+      <c r="A75" s="9">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B75" s="2"/>
-      <c r="C75" s="20"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="19"/>
       <c r="D75" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E75" s="2"/>
+      <c r="E75" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
+      <c r="A76" s="9">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="20"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="19"/>
       <c r="D76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E76" s="2"/>
+      <c r="E76" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="A77" s="9">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B77" s="2"/>
-      <c r="C77" s="20"/>
+      <c r="B77" s="26"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E77" s="2"/>
+      <c r="E77" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2">
+      <c r="A78" s="9">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B78" s="2"/>
-      <c r="C78" s="20"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E78" s="2"/>
+      <c r="E78" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2">
+      <c r="A79" s="9">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B79" s="2"/>
-      <c r="C79" s="20"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="19"/>
       <c r="D79" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2">
+      <c r="A80" s="9">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="20" t="s">
+      <c r="B80" s="26"/>
+      <c r="C80" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E80" s="2"/>
+      <c r="E80" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
+      <c r="A81" s="9">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B81" s="2"/>
-      <c r="C81" s="20"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="19"/>
       <c r="D81" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E81" s="2"/>
+      <c r="E81" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+      <c r="A82" s="9">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B82" s="2"/>
-      <c r="C82" s="20"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="19"/>
       <c r="D82" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E82" s="2"/>
+      <c r="E82" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="A83" s="9">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="20"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="19"/>
       <c r="D83" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E83" s="2"/>
+      <c r="E83" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="A84" s="9">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B84" s="2"/>
-      <c r="C84" s="20"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="19"/>
       <c r="D84" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E84" s="2"/>
+      <c r="E84" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
+      <c r="A85" s="9">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B85" s="2"/>
-      <c r="C85" s="20"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="19"/>
       <c r="D85" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="2"/>
+      <c r="E85" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="86" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="2">
+      <c r="A86" s="12">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="21"/>
-      <c r="D86" s="14" t="s">
+      <c r="B86" s="27"/>
+      <c r="C86" s="20"/>
+      <c r="D86" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E86" s="2"/>
+      <c r="E86" s="18" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
+      <c r="A87" s="6">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B87" s="2"/>
-      <c r="C87" s="19" t="s">
+      <c r="B87" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D87" s="8" t="s">
+      <c r="D87" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E87" s="2"/>
+      <c r="E87" s="30" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
+      <c r="A88" s="9">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="20"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="19"/>
       <c r="D88" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E88" s="2"/>
+      <c r="E88" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
+      <c r="A89" s="9">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B89" s="2"/>
-      <c r="C89" s="20"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="19"/>
       <c r="D89" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="2"/>
+      <c r="E89" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
+      <c r="A90" s="9">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B90" s="2"/>
-      <c r="C90" s="20"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="19"/>
       <c r="D90" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E90" s="2"/>
+      <c r="E90" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
+      <c r="A91" s="9">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B91" s="2"/>
-      <c r="C91" s="20"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="19"/>
       <c r="D91" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E91" s="2"/>
+      <c r="E91" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
+      <c r="A92" s="9">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B92" s="2"/>
-      <c r="C92" s="20"/>
+      <c r="B92" s="26"/>
+      <c r="C92" s="19"/>
       <c r="D92" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E92" s="2"/>
+      <c r="E92" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2">
+      <c r="A93" s="9">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B93" s="2"/>
-      <c r="C93" s="20"/>
+      <c r="B93" s="26"/>
+      <c r="C93" s="19"/>
       <c r="D93" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E93" s="2"/>
+      <c r="E93" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2">
+      <c r="A94" s="9">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B94" s="2"/>
-      <c r="C94" s="20"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="19"/>
       <c r="D94" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E94" s="2"/>
+      <c r="E94" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="2">
+      <c r="A95" s="9">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B95" s="2"/>
-      <c r="C95" s="20" t="s">
+      <c r="B95" s="26"/>
+      <c r="C95" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E95" s="2"/>
+      <c r="E95" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="2">
+      <c r="A96" s="9">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B96" s="2"/>
-      <c r="C96" s="20"/>
+      <c r="B96" s="26"/>
+      <c r="C96" s="19"/>
       <c r="D96" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E96" s="2"/>
+      <c r="E96" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="2">
+      <c r="A97" s="9">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B97" s="2"/>
-      <c r="C97" s="20"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="19"/>
       <c r="D97" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E97" s="2"/>
+      <c r="E97" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="2">
+      <c r="A98" s="9">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B98" s="2"/>
-      <c r="C98" s="20"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="19"/>
       <c r="D98" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E98" s="2"/>
+      <c r="E98" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="2">
+      <c r="A99" s="9">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="20"/>
+      <c r="B99" s="26"/>
+      <c r="C99" s="19"/>
       <c r="D99" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E99" s="2"/>
+      <c r="E99" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2">
+      <c r="A100" s="9">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="20"/>
+      <c r="B100" s="26"/>
+      <c r="C100" s="19"/>
       <c r="D100" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E100" s="2"/>
+      <c r="E100" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="2">
+      <c r="A101" s="9">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B101" s="2"/>
-      <c r="C101" s="20" t="s">
+      <c r="B101" s="26"/>
+      <c r="C101" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E101" s="2"/>
+      <c r="E101" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="2">
+      <c r="A102" s="9">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="20"/>
+      <c r="B102" s="26"/>
+      <c r="C102" s="19"/>
       <c r="D102" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E102" s="2"/>
+      <c r="E102" s="10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="2">
+      <c r="A103" s="9">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="20"/>
+      <c r="B103" s="26"/>
+      <c r="C103" s="19"/>
       <c r="D103" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E103" s="2"/>
+      <c r="E103" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="2">
+      <c r="A104" s="9">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B104" s="2"/>
-      <c r="C104" s="20"/>
+      <c r="B104" s="26"/>
+      <c r="C104" s="19"/>
       <c r="D104" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E104" s="2"/>
+      <c r="E104" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="2">
+      <c r="A105" s="9">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B105" s="2"/>
-      <c r="C105" s="20"/>
+      <c r="B105" s="26"/>
+      <c r="C105" s="19"/>
       <c r="D105" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E105" s="2"/>
+      <c r="E105" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="2">
+      <c r="A106" s="9">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B106" s="2"/>
-      <c r="C106" s="20"/>
+      <c r="B106" s="26"/>
+      <c r="C106" s="19"/>
       <c r="D106" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E106" s="2"/>
+      <c r="E106" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="107" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="2">
+      <c r="A107" s="12">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="B107" s="2"/>
-      <c r="C107" s="21"/>
-      <c r="D107" s="14" t="s">
+      <c r="B107" s="27"/>
+      <c r="C107" s="20"/>
+      <c r="D107" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="2"/>
+      <c r="E107" s="32" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="2">
+      <c r="A108" s="6">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="B108" s="2"/>
-      <c r="C108" s="19" t="s">
+      <c r="B108" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D108" s="8" t="s">
+      <c r="D108" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E108" s="2"/>
+      <c r="E108" s="30" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="2">
+      <c r="A109" s="9">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="B109" s="2"/>
-      <c r="C109" s="20"/>
+      <c r="B109" s="26"/>
+      <c r="C109" s="19"/>
       <c r="D109" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E109" s="2"/>
+      <c r="E109" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="2">
+      <c r="A110" s="9">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B110" s="2"/>
-      <c r="C110" s="20"/>
+      <c r="B110" s="26"/>
+      <c r="C110" s="19"/>
       <c r="D110" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="2">
+      <c r="A111" s="9">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="20"/>
+      <c r="B111" s="26"/>
+      <c r="C111" s="19"/>
       <c r="D111" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E111" s="2"/>
+      <c r="E111" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="2">
+      <c r="A112" s="9">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B112" s="2"/>
-      <c r="C112" s="20"/>
+      <c r="B112" s="26"/>
+      <c r="C112" s="19"/>
       <c r="D112" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E112" s="2"/>
+      <c r="E112" s="11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="2">
+      <c r="A113" s="9">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="20"/>
+      <c r="B113" s="26"/>
+      <c r="C113" s="19"/>
       <c r="D113" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E113" s="2"/>
+      <c r="E113" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="2">
+      <c r="A114" s="9">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="B114" s="2"/>
-      <c r="C114" s="20"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="19"/>
       <c r="D114" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E114" s="2"/>
+      <c r="E114" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="2">
+      <c r="A115" s="9">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B115" s="2"/>
-      <c r="C115" s="20"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="19"/>
       <c r="D115" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E115" s="2"/>
+      <c r="E115" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="2">
+      <c r="A116" s="9">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="20" t="s">
+      <c r="B116" s="26"/>
+      <c r="C116" s="19" t="s">
         <v>10</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E116" s="2"/>
+      <c r="E116" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="2">
+      <c r="A117" s="9">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="B117" s="2"/>
-      <c r="C117" s="20"/>
+      <c r="B117" s="26"/>
+      <c r="C117" s="19"/>
       <c r="D117" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E117" s="2"/>
+      <c r="E117" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="2">
+      <c r="A118" s="9">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="B118" s="2"/>
-      <c r="C118" s="20"/>
+      <c r="B118" s="26"/>
+      <c r="C118" s="19"/>
       <c r="D118" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="2"/>
+      <c r="E118" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="2">
+      <c r="A119" s="9">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="B119" s="2"/>
-      <c r="C119" s="20"/>
+      <c r="B119" s="26"/>
+      <c r="C119" s="19"/>
       <c r="D119" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E119" s="2"/>
+      <c r="E119" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="2">
+      <c r="A120" s="9">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="B120" s="2"/>
-      <c r="C120" s="20"/>
+      <c r="B120" s="26"/>
+      <c r="C120" s="19"/>
       <c r="D120" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E120" s="2"/>
+      <c r="E120" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="2">
+      <c r="A121" s="9">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B121" s="17"/>
-      <c r="C121" s="20"/>
+      <c r="B121" s="26"/>
+      <c r="C121" s="19"/>
       <c r="D121" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E121" s="2"/>
+      <c r="E121" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="24">
+      <c r="A122" s="28">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B122" s="2"/>
-      <c r="C122" s="25" t="s">
+      <c r="B122" s="26"/>
+      <c r="C122" s="22" t="s">
         <v>11</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E122" s="2"/>
+      <c r="E122" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="24">
+      <c r="A123" s="28">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="25"/>
+      <c r="B123" s="26"/>
+      <c r="C123" s="22"/>
       <c r="D123" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E123" s="2"/>
+      <c r="E123" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="24">
+      <c r="A124" s="28">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="B124" s="2"/>
-      <c r="C124" s="25"/>
+      <c r="B124" s="26"/>
+      <c r="C124" s="22"/>
       <c r="D124" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E124" s="2"/>
+      <c r="E124" s="11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="24">
+      <c r="A125" s="28">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="B125" s="2"/>
-      <c r="C125" s="25"/>
+      <c r="B125" s="26"/>
+      <c r="C125" s="22"/>
       <c r="D125" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E125" s="2"/>
+      <c r="E125" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="24">
+      <c r="A126" s="28">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="B126" s="2"/>
-      <c r="C126" s="25"/>
+      <c r="B126" s="26"/>
+      <c r="C126" s="22"/>
       <c r="D126" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E126" s="2"/>
+      <c r="E126" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="24">
+      <c r="A127" s="28">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="B127" s="2"/>
-      <c r="C127" s="25"/>
+      <c r="B127" s="26"/>
+      <c r="C127" s="22"/>
       <c r="D127" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E127" s="2"/>
+      <c r="E127" s="31" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="128" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="24">
+      <c r="A128" s="29">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="B128" s="2"/>
-      <c r="C128" s="26"/>
-      <c r="D128" s="14" t="s">
+      <c r="B128" s="27"/>
+      <c r="C128" s="23"/>
+      <c r="D128" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="E128" s="2"/>
+      <c r="E128" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="24">
+    <mergeCell ref="B66:B86"/>
+    <mergeCell ref="B87:B107"/>
+    <mergeCell ref="B108:B128"/>
+    <mergeCell ref="C45:C52"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="C59:C65"/>
+    <mergeCell ref="B45:B65"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="B24:B44"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="C11:C16"/>
+    <mergeCell ref="C17:C23"/>
+    <mergeCell ref="B3:B23"/>
+    <mergeCell ref="C24:C31"/>
     <mergeCell ref="C101:C107"/>
     <mergeCell ref="C108:C115"/>
     <mergeCell ref="C116:C121"/>
@@ -2573,18 +2799,6 @@
     <mergeCell ref="C80:C86"/>
     <mergeCell ref="C87:C94"/>
     <mergeCell ref="C95:C100"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="C11:C16"/>
-    <mergeCell ref="C17:C23"/>
-    <mergeCell ref="B3:B23"/>
-    <mergeCell ref="C24:C31"/>
-    <mergeCell ref="C45:C52"/>
-    <mergeCell ref="C53:C58"/>
-    <mergeCell ref="C59:C65"/>
-    <mergeCell ref="B45:B65"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="C38:C44"/>
-    <mergeCell ref="B24:B44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>